<commit_message>
more work on bambatsi validation set
</commit_message>
<xml_diff>
--- a/Prototypes/Bambatsi/Observed.xlsx
+++ b/Prototypes/Bambatsi/Observed.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Bambatsi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Bambatsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="ObservedSoilWater" sheetId="2" r:id="rId2"/>
     <sheet name="HudsonRunoff" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="23">
   <si>
     <t>B_LAI</t>
   </si>
@@ -71,22 +71,31 @@
     <t>DeadBiomass</t>
   </si>
   <si>
-    <t>SW10_110cm</t>
+    <t>SW10_50cm</t>
   </si>
   <si>
-    <t>SW110_210cm</t>
+    <t>SW50_90cm</t>
   </si>
   <si>
-    <t>SW210_310cm</t>
+    <t>SW90_130cm</t>
   </si>
   <si>
-    <t>SW10_310cm</t>
+    <t>SW130_170cm</t>
+  </si>
+  <si>
+    <t>SW170_210cm</t>
+  </si>
+  <si>
+    <t>SW210_250cm</t>
+  </si>
+  <si>
+    <t>SW10_250cm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -157,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -166,6 +175,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,23 +269,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -311,23 +304,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -486,16 +462,16 @@
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.38671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -533,7 +509,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -575,7 +551,7 @@
         <v>279.125</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -617,7 +593,7 @@
         <v>464.73749928706059</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -660,7 +636,7 @@
         <v>1177.2591667905765</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -703,7 +679,7 @@
         <v>1328.827501313991</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -746,7 +722,7 @@
         <v>1328.827501313991</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -789,7 +765,7 @@
         <v>1328.827501313991</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -832,7 +808,7 @@
         <v>1465.1168150967485</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -875,7 +851,7 @@
         <v>1642.538915422381</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -918,7 +894,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -961,7 +937,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +980,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1047,7 +1023,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1090,7 +1066,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1133,7 +1109,7 @@
         <v>2021.7713279289001</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1176,7 +1152,7 @@
         <v>2021.7713279289001</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1195,7 @@
         <v>2220.7840767706889</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1262,7 +1238,7 @@
         <v>2220.7840767706889</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1305,7 +1281,7 @@
         <v>2220.7840767706889</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1348,7 +1324,7 @@
         <v>2461.4965271048768</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1391,7 +1367,7 @@
         <v>2586.6707063880876</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1434,7 +1410,7 @@
         <v>2623.7996456745291</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1477,7 +1453,7 @@
         <v>2654.7762397534466</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1520,7 +1496,7 @@
         <v>2654.7762397534466</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1563,7 +1539,7 @@
         <v>2899.8972279812174</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1616,18 +1592,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1646,1345 +1626,2024 @@
       <c r="F1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="8">
         <v>34690</v>
       </c>
       <c r="C2">
-        <v>484.06909093690774</v>
+        <v>198.58459999999999</v>
       </c>
       <c r="D2">
-        <v>437.60353057508428</v>
+        <v>194.2424</v>
       </c>
       <c r="E2">
-        <v>419.17111708750588</v>
+        <v>180.5471</v>
       </c>
       <c r="F2">
-        <v>1340.843738599498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+        <v>178.2758</v>
+      </c>
+      <c r="G2">
+        <v>170.02279999999999</v>
+      </c>
+      <c r="H2">
+        <v>166.40459999999999</v>
+      </c>
+      <c r="I2">
+        <f>SUM(C2:H2)</f>
+        <v>1088.0772999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="8">
         <v>34712</v>
       </c>
       <c r="C3">
-        <v>497.14566232490745</v>
+        <v>205.624</v>
       </c>
       <c r="D3">
-        <v>443.57392249569375</v>
+        <v>198.9393</v>
       </c>
       <c r="E3">
-        <v>422.26924424497122</v>
+        <v>183.4282</v>
       </c>
       <c r="F3">
-        <v>1362.9888290655722</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+        <v>180.25210000000001</v>
+      </c>
+      <c r="G3">
+        <v>172.476</v>
+      </c>
+      <c r="H3">
+        <v>167.7062</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I66" si="0">SUM(C3:H3)</f>
+        <v>1108.4258000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>34732</v>
       </c>
       <c r="C4">
-        <v>500.89797385639361</v>
+        <v>206.90360000000001</v>
       </c>
       <c r="D4">
-        <v>447.48505588151136</v>
+        <v>200.9281</v>
       </c>
       <c r="E4">
-        <v>424.82006118814223</v>
+        <v>184.62739999999999</v>
       </c>
       <c r="F4">
-        <v>1373.203090926047</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+        <v>181.3843</v>
+      </c>
+      <c r="G4">
+        <v>174.53970000000001</v>
+      </c>
+      <c r="H4">
+        <v>167.82679999999999</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>1116.2099000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="8">
         <v>34746</v>
       </c>
       <c r="C5">
-        <v>489.45982444423851</v>
+        <v>197.4984</v>
       </c>
       <c r="D5">
-        <v>442.77612537577431</v>
+        <v>199.23820000000001</v>
       </c>
       <c r="E5">
-        <v>423.99786148678265</v>
+        <v>183.09710000000001</v>
       </c>
       <c r="F5">
-        <v>1356.2338113067954</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+        <v>180.37540000000001</v>
+      </c>
+      <c r="G5">
+        <v>172.02699999999999</v>
+      </c>
+      <c r="H5">
+        <v>168.13040000000001</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>1100.3665000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>34760</v>
       </c>
       <c r="C6">
-        <v>476.06734296068907</v>
+        <v>189.6541</v>
       </c>
       <c r="D6">
-        <v>451.43825374501364</v>
+        <v>194.03059999999999</v>
       </c>
       <c r="E6">
-        <v>428.91369668588652</v>
+        <v>183.43799999999999</v>
       </c>
       <c r="F6">
-        <v>1356.4192933915892</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+        <v>182.86099999999999</v>
+      </c>
+      <c r="G6">
+        <v>177.52180000000001</v>
+      </c>
+      <c r="H6">
+        <v>170.3828</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>1097.8883000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="8">
         <v>34774</v>
       </c>
       <c r="C7">
-        <v>449.49152553099429</v>
+        <v>167.14320000000001</v>
       </c>
       <c r="D7">
-        <v>451.86823971450667</v>
+        <v>188.6865</v>
       </c>
       <c r="E7">
-        <v>430.6807267670327</v>
+        <v>186.10380000000001</v>
       </c>
       <c r="F7">
-        <v>1332.0404920125338</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+        <v>183.5745</v>
+      </c>
+      <c r="G7">
+        <v>175.8518</v>
+      </c>
+      <c r="H7">
+        <v>169.56399999999999</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>1070.9238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <v>34788</v>
       </c>
       <c r="C8">
-        <v>421.25995102147374</v>
+        <v>154.33330000000001</v>
       </c>
       <c r="D8">
-        <v>453.03873546726015</v>
+        <v>176.10079999999999</v>
       </c>
       <c r="E8">
-        <v>434.42921482769015</v>
+        <v>181.91810000000001</v>
       </c>
       <c r="F8">
-        <v>1308.7279013164243</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+        <v>183.5909</v>
+      </c>
+      <c r="G8">
+        <v>178.35560000000001</v>
+      </c>
+      <c r="H8">
+        <v>172.08449999999999</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1046.3832</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="8">
         <v>34802</v>
       </c>
       <c r="C9">
-        <v>403.0598898085546</v>
+        <v>144.02279999999999</v>
       </c>
       <c r="D9">
-        <v>449.68556753497603</v>
+        <v>170.7893</v>
       </c>
       <c r="E9">
-        <v>432.95123822521111</v>
+        <v>177.54220000000001</v>
       </c>
       <c r="F9">
-        <v>1285.6966955687417</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+        <v>183.0829</v>
+      </c>
+      <c r="G9">
+        <v>177.3081</v>
+      </c>
+      <c r="H9">
+        <v>170.2817</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>1023.0269999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="8">
         <v>34830</v>
       </c>
       <c r="C10">
-        <v>390.81296639800928</v>
+        <v>137.97929999999999</v>
       </c>
       <c r="D10">
-        <v>443.9918156577948</v>
+        <v>166.1901</v>
       </c>
       <c r="E10">
-        <v>432.00367326443472</v>
+        <v>174.51570000000001</v>
       </c>
       <c r="F10">
-        <v>1266.8084553202389</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+        <v>179.7235</v>
+      </c>
+      <c r="G10">
+        <v>176.39619999999999</v>
+      </c>
+      <c r="H10">
+        <v>170.48259999999999</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>1005.2873999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="8">
         <v>34848</v>
       </c>
       <c r="C11">
-        <v>452.07519463808069</v>
+        <v>186.97309999999999</v>
       </c>
       <c r="D11">
-        <v>449.34190186395756</v>
+        <v>177.2722</v>
       </c>
       <c r="E11">
-        <v>444.95488886597866</v>
+        <v>176.66069999999999</v>
       </c>
       <c r="F11">
-        <v>1346.3719853680168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+        <v>180.94919999999999</v>
+      </c>
+      <c r="G11">
+        <v>179.56200000000001</v>
+      </c>
+      <c r="H11">
+        <v>174.7826</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1076.1997999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="8">
         <v>34876</v>
       </c>
       <c r="C12">
-        <v>446.08416596552661</v>
+        <v>184.16749999999999</v>
       </c>
       <c r="D12">
-        <v>447.09976211348129</v>
+        <v>174.43780000000001</v>
       </c>
       <c r="E12">
-        <v>440.90565200684688</v>
+        <v>176.0804</v>
       </c>
       <c r="F12">
-        <v>1334.0895800858548</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+        <v>180.32259999999999</v>
+      </c>
+      <c r="G12">
+        <v>178.17570000000001</v>
+      </c>
+      <c r="H12">
+        <v>173.6977</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>1066.8816999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="8">
         <v>34905</v>
       </c>
       <c r="C13">
-        <v>437.98388340232958</v>
+        <v>176.73939999999999</v>
       </c>
       <c r="D13">
-        <v>445.01744830277192</v>
+        <v>174.08320000000001</v>
       </c>
       <c r="E13">
-        <v>436.51828711454743</v>
+        <v>175.37360000000001</v>
       </c>
       <c r="F13">
-        <v>1319.5196188196489</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+        <v>179.922</v>
+      </c>
+      <c r="G13">
+        <v>176.88310000000001</v>
+      </c>
+      <c r="H13">
+        <v>171.7807</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>1054.7819999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="8">
         <v>34941</v>
       </c>
       <c r="C14">
-        <v>415.97563907819506</v>
+        <v>158.45939999999999</v>
       </c>
       <c r="D14">
-        <v>444.51233150135084</v>
+        <v>170.6079</v>
       </c>
       <c r="E14">
-        <v>436.96904485408277</v>
+        <v>174.9939</v>
       </c>
       <c r="F14">
-        <v>1297.4570154336286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+        <v>179.55690000000001</v>
+      </c>
+      <c r="G14">
+        <v>176.8698</v>
+      </c>
+      <c r="H14">
+        <v>172.13919999999999</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>1032.6271000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="8">
         <v>34969</v>
       </c>
       <c r="C15">
-        <v>407.69876446403362</v>
+        <v>160.554</v>
       </c>
       <c r="D15">
-        <v>437.85973520991763</v>
+        <v>162.70400000000001</v>
       </c>
       <c r="E15">
-        <v>430.41004306771009</v>
+        <v>171.10300000000001</v>
       </c>
       <c r="F15">
-        <v>1275.9685427416614</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+        <v>177.2422</v>
+      </c>
+      <c r="G15">
+        <v>173.95529999999999</v>
+      </c>
+      <c r="H15">
+        <v>169.77350000000001</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>1015.332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="8">
         <v>35004</v>
       </c>
       <c r="C16">
-        <v>378.95882404574434</v>
+        <v>141.9076</v>
       </c>
       <c r="D16">
-        <v>424.54128742405419</v>
+        <v>155.85040000000001</v>
       </c>
       <c r="E16">
-        <v>420.19837415281307</v>
+        <v>164.791</v>
       </c>
       <c r="F16">
-        <v>1223.6984856226118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+        <v>172.4152</v>
+      </c>
+      <c r="G16">
+        <v>168.536</v>
+      </c>
+      <c r="H16">
+        <v>164.44280000000001</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>967.94299999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="8">
         <v>35033</v>
       </c>
       <c r="C17">
-        <v>387.34959501364659</v>
+        <v>153.37450000000001</v>
       </c>
       <c r="D17">
-        <v>420.56481398127323</v>
+        <v>154.1242</v>
       </c>
       <c r="E17">
-        <v>420.16409769647953</v>
+        <v>162.08260000000001</v>
       </c>
       <c r="F17">
-        <v>1228.0785066913995</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+        <v>170.14420000000001</v>
+      </c>
+      <c r="G17">
+        <v>168.18879999999999</v>
+      </c>
+      <c r="H17">
+        <v>164.09649999999999</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>972.01080000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="8">
         <v>35074</v>
       </c>
       <c r="C18">
-        <v>472.24132826560208</v>
+        <v>195.977</v>
       </c>
       <c r="D18">
-        <v>435.75265507665029</v>
+        <v>187.23679999999999</v>
       </c>
       <c r="E18">
-        <v>428.7244792854234</v>
+        <v>176.94569999999999</v>
       </c>
       <c r="F18">
-        <v>1336.7184626276758</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+        <v>176.68680000000001</v>
+      </c>
+      <c r="G18">
+        <v>171.14769999999999</v>
+      </c>
+      <c r="H18">
+        <v>168.3828</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>1076.3768</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="8">
         <v>35104</v>
       </c>
       <c r="C19">
-        <v>475.60732593577893</v>
+        <v>200.67150000000001</v>
       </c>
       <c r="D19">
-        <v>433.52769989511683</v>
+        <v>186.6782</v>
       </c>
       <c r="E19">
-        <v>430.69180900725894</v>
+        <v>175.62039999999999</v>
       </c>
       <c r="F19">
-        <v>1339.8268348381546</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+        <v>175.6944</v>
+      </c>
+      <c r="G19">
+        <v>170.47049999999999</v>
+      </c>
+      <c r="H19">
+        <v>168.0881</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>1077.2230999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="8">
         <v>35131</v>
       </c>
       <c r="C20">
-        <v>411.50430837260285</v>
+        <v>152.4537</v>
       </c>
       <c r="D20">
-        <v>435.15327213613875</v>
+        <v>172.25819999999999</v>
       </c>
       <c r="E20">
-        <v>428.88738314954145</v>
+        <v>174.2396</v>
       </c>
       <c r="F20">
-        <v>1275.544963658283</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+        <v>175.8554</v>
+      </c>
+      <c r="G20">
+        <v>171.85069999999999</v>
+      </c>
+      <c r="H20">
+        <v>167.93870000000001</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>1014.5963</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="8">
         <v>35153</v>
       </c>
       <c r="C21">
-        <v>378.27068099876885</v>
+        <v>134.80619999999999</v>
       </c>
       <c r="D21">
-        <v>429.05428530153188</v>
+        <v>160.4041</v>
       </c>
       <c r="E21">
-        <v>426.97824297456583</v>
+        <v>167.94030000000001</v>
       </c>
       <c r="F21">
-        <v>1234.3032092748667</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+        <v>173.79130000000001</v>
+      </c>
+      <c r="G21">
+        <v>170.38300000000001</v>
+      </c>
+      <c r="H21">
+        <v>166.54640000000001</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>973.87130000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="8">
         <v>35200</v>
       </c>
       <c r="C22">
-        <v>371.41809157682559</v>
+        <v>139.8777</v>
       </c>
       <c r="D22">
-        <v>420.50385594051869</v>
+        <v>151.9907</v>
       </c>
       <c r="E22">
-        <v>427.4207085990389</v>
+        <v>161.9042</v>
       </c>
       <c r="F22">
-        <v>1219.3426561163833</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+        <v>170.0771</v>
+      </c>
+      <c r="G22">
+        <v>168.07220000000001</v>
+      </c>
+      <c r="H22">
+        <v>167.47900000000001</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>959.40090000000009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="8">
         <v>35224</v>
       </c>
       <c r="C23">
-        <v>365.68346047494663</v>
+        <v>134.6687</v>
       </c>
       <c r="D23">
-        <v>419.49557227708482</v>
+        <v>151.91059999999999</v>
       </c>
       <c r="E23">
-        <v>427.14826250115567</v>
+        <v>160.95779999999999</v>
       </c>
       <c r="F23">
-        <v>1212.327295253187</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+        <v>170.0907</v>
+      </c>
+      <c r="G23">
+        <v>167.55119999999999</v>
+      </c>
+      <c r="H23">
+        <v>166.77080000000001</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>951.94979999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="8">
         <v>35257</v>
       </c>
       <c r="C24">
-        <v>367.59431449067085</v>
+        <v>139.54949999999999</v>
       </c>
       <c r="D24">
-        <v>415.77081063000804</v>
+        <v>149.857</v>
       </c>
       <c r="E24">
-        <v>421.31513483653441</v>
+        <v>159.21780000000001</v>
       </c>
       <c r="F24">
-        <v>1204.6802599572134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+        <v>168.2705</v>
+      </c>
+      <c r="G24">
+        <v>166.47030000000001</v>
+      </c>
+      <c r="H24">
+        <v>163.86070000000001</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>947.22579999999994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="8">
         <v>35298</v>
       </c>
       <c r="C25">
-        <v>414.11709398947113</v>
+        <v>174.3794</v>
       </c>
       <c r="D25">
-        <v>421.11328132718489</v>
+        <v>160.01740000000001</v>
       </c>
       <c r="E25">
-        <v>430.65265676604957</v>
+        <v>161.70820000000001</v>
       </c>
       <c r="F25">
-        <v>1265.8830320827055</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+        <v>170.1729</v>
+      </c>
+      <c r="G25">
+        <v>168.95249999999999</v>
+      </c>
+      <c r="H25">
+        <v>166.66630000000001</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>1001.8967</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="8">
         <v>35328</v>
       </c>
       <c r="C26">
-        <v>444.49023639325503</v>
+        <v>181.726</v>
       </c>
       <c r="D26">
-        <v>425.60133909049603</v>
+        <v>177.6713</v>
       </c>
       <c r="E26">
-        <v>423.13193983136773</v>
+        <v>170.44589999999999</v>
       </c>
       <c r="F26">
-        <v>1293.2235153151191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+        <v>172.78460000000001</v>
+      </c>
+      <c r="G26">
+        <v>167.46379999999999</v>
+      </c>
+      <c r="H26">
+        <v>164.71719999999999</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>1034.8088</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="8">
         <v>35362</v>
       </c>
       <c r="C27">
-        <v>432.91294897987621</v>
+        <v>172.48070000000001</v>
       </c>
       <c r="D27">
-        <v>428.76567334360544</v>
+        <v>175.48050000000001</v>
       </c>
       <c r="E27">
-        <v>424.93008665204604</v>
+        <v>170.49979999999999</v>
       </c>
       <c r="F27">
-        <v>1286.6087089755279</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+        <v>174.15620000000001</v>
+      </c>
+      <c r="G27">
+        <v>169.06139999999999</v>
+      </c>
+      <c r="H27">
+        <v>165.3314</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>1027.01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="8">
         <v>35404</v>
       </c>
       <c r="C28">
-        <v>346.5764389442993</v>
+        <v>122.9708</v>
       </c>
       <c r="D28">
-        <v>414.14707274350366</v>
+        <v>146.37799999999999</v>
       </c>
       <c r="E28">
-        <v>417.13863354062175</v>
+        <v>157.66759999999999</v>
       </c>
       <c r="F28">
-        <v>1177.8621452284247</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+        <v>168.14689999999999</v>
+      </c>
+      <c r="G28">
+        <v>165.56030000000001</v>
+      </c>
+      <c r="H28">
+        <v>162.4863</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>923.20989999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="8">
         <v>35443</v>
       </c>
       <c r="C29">
-        <v>374.64129183386962</v>
+        <v>138.17439999999999</v>
       </c>
       <c r="D29">
-        <v>413.66381380726068</v>
+        <v>156.73689999999999</v>
       </c>
       <c r="E29">
-        <v>415.49164742330487</v>
+        <v>160.97999999999999</v>
       </c>
       <c r="F29">
-        <v>1203.7967530644353</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+        <v>167.42150000000001</v>
+      </c>
+      <c r="G29">
+        <v>164.9923</v>
+      </c>
+      <c r="H29">
+        <v>162.27449999999999</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>950.57960000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="8">
         <v>35467</v>
       </c>
       <c r="C30">
-        <v>470.95790188950161</v>
+        <v>193.76570000000001</v>
       </c>
       <c r="D30">
-        <v>421.70821551532219</v>
+        <v>188.79839999999999</v>
       </c>
       <c r="E30">
-        <v>412.00319755859857</v>
+        <v>175.30930000000001</v>
       </c>
       <c r="F30">
-        <v>1304.6693149634225</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+        <v>171.49520000000001</v>
+      </c>
+      <c r="G30">
+        <v>163.29769999999999</v>
+      </c>
+      <c r="H30">
+        <v>159.89169999999999</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>1052.558</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="8">
         <v>35482</v>
       </c>
       <c r="C31">
-        <v>444.85744401151703</v>
+        <v>178.13919999999999</v>
       </c>
       <c r="D31">
-        <v>421.44060201925976</v>
+        <v>180.05330000000001</v>
       </c>
       <c r="E31">
-        <v>411.56805194483132</v>
+        <v>172.58600000000001</v>
       </c>
       <c r="F31">
-        <v>1277.8660979756082</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+        <v>170.96780000000001</v>
+      </c>
+      <c r="G31">
+        <v>164.55170000000001</v>
+      </c>
+      <c r="H31">
+        <v>160.327</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>1026.625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="8">
         <v>35503</v>
       </c>
       <c r="C32">
-        <v>373.75727821861312</v>
+        <v>135.0624</v>
       </c>
       <c r="D32">
-        <v>416.53909942062154</v>
+        <v>157.67529999999999</v>
       </c>
       <c r="E32">
-        <v>411.76010783452131</v>
+        <v>163.91739999999999</v>
       </c>
       <c r="F32">
-        <v>1202.0564854737559</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+        <v>169.22909999999999</v>
+      </c>
+      <c r="G32">
+        <v>164.41220000000001</v>
+      </c>
+      <c r="H32">
+        <v>160.46379999999999</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>950.76019999999994</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="8">
         <v>35542</v>
       </c>
       <c r="C33">
-        <v>319.55455510128957</v>
+        <v>108.8022</v>
       </c>
       <c r="D33">
-        <v>398.45195962674461</v>
+        <v>137.8323</v>
       </c>
       <c r="E33">
-        <v>408.64331854792454</v>
+        <v>149.1978</v>
       </c>
       <c r="F33">
-        <v>1126.6498332759588</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+        <v>161.2227</v>
+      </c>
+      <c r="G33">
+        <v>160.95140000000001</v>
+      </c>
+      <c r="H33">
+        <v>158.37219999999999</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>876.37860000000012</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="8">
         <v>35579</v>
       </c>
       <c r="C34">
-        <v>322.33547085161985</v>
+        <v>114.9213</v>
       </c>
       <c r="D34">
-        <v>397.01690080863847</v>
+        <v>135.22470000000001</v>
       </c>
       <c r="E34">
-        <v>415.56690815710419</v>
+        <v>147.75880000000001</v>
       </c>
       <c r="F34">
-        <v>1134.9192798173624</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+        <v>160.76660000000001</v>
+      </c>
+      <c r="G34">
+        <v>160.68090000000001</v>
+      </c>
+      <c r="H34">
+        <v>160.06280000000001</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>879.41510000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="8">
         <v>35605</v>
       </c>
       <c r="C35">
-        <v>320.99564044814605</v>
+        <v>114.5275</v>
       </c>
       <c r="D35">
-        <v>396.7125462183742</v>
+        <v>134.56479999999999</v>
       </c>
       <c r="E35">
-        <v>415.54819373080966</v>
+        <v>147.42089999999999</v>
       </c>
       <c r="F35">
-        <v>1133.2563803973298</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+        <v>160.5444</v>
+      </c>
+      <c r="G35">
+        <v>160.6507</v>
+      </c>
+      <c r="H35">
+        <v>160.852</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>878.56029999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="8">
         <v>35634</v>
       </c>
       <c r="C36">
-        <v>321.61656790654854</v>
+        <v>113.9104</v>
       </c>
       <c r="D36">
-        <v>399.29048905077434</v>
+        <v>135.2165</v>
       </c>
       <c r="E36">
-        <v>423.1688932611454</v>
+        <v>148.429</v>
       </c>
       <c r="F36">
-        <v>1144.0759502184683</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+        <v>161.31120000000001</v>
+      </c>
+      <c r="G36">
+        <v>162.03989999999999</v>
+      </c>
+      <c r="H36">
+        <v>162.7038</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>883.61079999999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="8">
         <v>35669</v>
       </c>
       <c r="C37">
-        <v>318.40370444921467</v>
+        <v>113.026</v>
       </c>
       <c r="D37">
-        <v>400.46447690301994</v>
+        <v>133.24979999999999</v>
       </c>
       <c r="E37">
-        <v>431.65752119643713</v>
+        <v>148.19370000000001</v>
       </c>
       <c r="F37">
-        <v>1150.5257025486717</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+        <v>162.27799999999999</v>
+      </c>
+      <c r="G37">
+        <v>162.1207</v>
+      </c>
+      <c r="H37">
+        <v>163.02799999999999</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>881.89620000000014</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="8">
         <v>35702</v>
       </c>
       <c r="C38">
-        <v>320.52082314861417</v>
+        <v>124.0677</v>
       </c>
       <c r="D38">
-        <v>374.05809154592089</v>
+        <v>128.39940000000001</v>
       </c>
       <c r="E38">
-        <v>383.55063845704666</v>
+        <v>139.50579999999999</v>
       </c>
       <c r="F38">
-        <v>1078.1295531515816</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+        <v>152.2336</v>
+      </c>
+      <c r="G38">
+        <v>150.3724</v>
+      </c>
+      <c r="H38">
+        <v>148.30160000000001</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>842.88049999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="8">
         <v>35726</v>
       </c>
       <c r="C39">
-        <v>319.230345859051</v>
+        <v>117.5628</v>
       </c>
       <c r="D39">
-        <v>381.14432037988786</v>
+        <v>132.02379999999999</v>
       </c>
       <c r="E39">
-        <v>387.78143906665554</v>
+        <v>142.5479</v>
       </c>
       <c r="F39">
-        <v>1088.1561053055943</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+        <v>154.98689999999999</v>
+      </c>
+      <c r="G39">
+        <v>153.25319999999999</v>
+      </c>
+      <c r="H39">
+        <v>150.66589999999999</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>851.04049999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="8">
         <v>35768</v>
       </c>
       <c r="C40">
-        <v>296.64690612198302</v>
+        <v>101.95059999999999</v>
       </c>
       <c r="D40">
-        <v>379.43727295432461</v>
+        <v>126.7647</v>
       </c>
       <c r="E40">
-        <v>396.26703590949307</v>
+        <v>139.5746</v>
       </c>
       <c r="F40">
-        <v>1072.3512149858007</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+        <v>154.13570000000001</v>
+      </c>
+      <c r="G40">
+        <v>153.65860000000001</v>
+      </c>
+      <c r="H40">
+        <v>153.56379999999999</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>829.64800000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="8">
         <v>35786</v>
       </c>
       <c r="C41">
-        <v>306.701362615731</v>
+        <v>110.79389999999999</v>
       </c>
       <c r="D41">
-        <v>380.48938005100518</v>
+        <v>127.99420000000001</v>
       </c>
       <c r="E41">
-        <v>397.09928359276233</v>
+        <v>139.79900000000001</v>
       </c>
       <c r="F41">
-        <v>1084.2900262594983</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+        <v>154.19049999999999</v>
+      </c>
+      <c r="G41">
+        <v>154.41309999999999</v>
+      </c>
+      <c r="H41">
+        <v>153.12010000000001</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>840.31079999999986</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="8">
         <v>35815</v>
       </c>
       <c r="C42">
-        <v>299.13786510570452</v>
+        <v>109.5415</v>
       </c>
       <c r="D42">
-        <v>374.02117680792156</v>
+        <v>123.6298</v>
       </c>
       <c r="E42">
-        <v>393.39079762621679</v>
+        <v>135.88</v>
       </c>
       <c r="F42">
-        <v>1066.5498395398429</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+        <v>151.87260000000001</v>
+      </c>
+      <c r="G42">
+        <v>152.23519999999999</v>
+      </c>
+      <c r="H42">
+        <v>151.71209999999999</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>824.87119999999993</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="8">
         <v>35850</v>
       </c>
       <c r="C43">
-        <v>303.26368859378653</v>
+        <v>111.2658</v>
       </c>
       <c r="D43">
-        <v>377.16071492817855</v>
+        <v>125.6611</v>
       </c>
       <c r="E43">
-        <v>391.5564684673451</v>
+        <v>137.01249999999999</v>
       </c>
       <c r="F43">
-        <v>1071.9808719893103</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+        <v>153.59549999999999</v>
+      </c>
+      <c r="G43">
+        <v>152.8896</v>
+      </c>
+      <c r="H43">
+        <v>150.86089999999999</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>831.28539999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="8">
         <v>35879</v>
       </c>
       <c r="C44">
-        <v>274.01697249057145</v>
+        <v>95.578400000000002</v>
       </c>
       <c r="D44">
-        <v>366.83532078534989</v>
+        <v>115.7771</v>
       </c>
       <c r="E44">
-        <v>386.54194050153728</v>
+        <v>130.35769999999999</v>
       </c>
       <c r="F44">
-        <v>1027.3942337774588</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+        <v>149.59200000000001</v>
+      </c>
+      <c r="G44">
+        <v>149.5471</v>
+      </c>
+      <c r="H44">
+        <v>148.1148</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>788.96710000000007</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="8">
         <v>35913</v>
       </c>
       <c r="C45">
-        <v>288.78943851662598</v>
+        <v>114.98180000000001</v>
       </c>
       <c r="D45">
-        <v>368.69955024039274</v>
+        <v>112.643</v>
       </c>
       <c r="E45">
-        <v>394.47744025258612</v>
+        <v>128.042</v>
       </c>
       <c r="F45">
-        <v>1051.9664290096048</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+        <v>149.9075</v>
+      </c>
+      <c r="G45">
+        <v>151.91470000000001</v>
+      </c>
+      <c r="H45">
+        <v>151.58940000000001</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>809.0784000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="8">
         <v>35940</v>
       </c>
       <c r="C46">
-        <v>351.48623180605273</v>
+        <v>159.8954</v>
       </c>
       <c r="D46">
-        <v>373.62539970151454</v>
+        <v>128.17689999999999</v>
       </c>
       <c r="E46">
-        <v>395.90250813204489</v>
+        <v>131.7311</v>
       </c>
       <c r="F46">
-        <v>1121.014139639612</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+        <v>151.8912</v>
+      </c>
+      <c r="G46">
+        <v>153.4171</v>
+      </c>
+      <c r="H46">
+        <v>151.59790000000001</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>876.70960000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="8">
         <v>35956</v>
       </c>
       <c r="C47">
-        <v>408.15488033128509</v>
+        <v>176.6224</v>
       </c>
       <c r="D47">
-        <v>382.54872914962772</v>
+        <v>159.05600000000001</v>
       </c>
       <c r="E47">
-        <v>395.22637003403918</v>
+        <v>146.02010000000001</v>
       </c>
       <c r="F47">
-        <v>1185.929979514952</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+        <v>155.8802</v>
+      </c>
+      <c r="G47">
+        <v>153.1249</v>
+      </c>
+      <c r="H47">
+        <v>151.3751</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>942.07870000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="8">
         <v>35979</v>
       </c>
       <c r="C48">
-        <v>462.79802609257951</v>
+        <v>190.4829</v>
       </c>
       <c r="D48">
-        <v>403.49088606387295</v>
+        <v>186.84639999999999</v>
       </c>
       <c r="E48">
-        <v>396.69000816727441</v>
+        <v>169.42410000000001</v>
       </c>
       <c r="F48">
-        <v>1262.9789203237269</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+        <v>166.0693</v>
+      </c>
+      <c r="G48">
+        <v>153.46619999999999</v>
+      </c>
+      <c r="H48">
+        <v>151.8312</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>1018.1201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="8">
         <v>36007</v>
       </c>
       <c r="C49">
-        <v>524.40336638351835</v>
+        <v>226.01240000000001</v>
       </c>
       <c r="D49">
-        <v>400.14355498971599</v>
+        <v>209.14869999999999</v>
       </c>
       <c r="E49">
-        <v>402.31216187417721</v>
+        <v>173.50989999999999</v>
       </c>
       <c r="F49">
-        <v>1326.8590832474115</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+        <v>163.33879999999999</v>
+      </c>
+      <c r="G49">
+        <v>152.53710000000001</v>
+      </c>
+      <c r="H49">
+        <v>153.0085</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="0"/>
+        <v>1077.5554</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="8">
         <v>36039</v>
       </c>
       <c r="C50">
-        <v>473.87146629426917</v>
+        <v>179.9126</v>
       </c>
       <c r="D50">
-        <v>405.3218692105184</v>
+        <v>203.4359</v>
       </c>
       <c r="E50">
-        <v>397.95568140478508</v>
+        <v>177.2157</v>
       </c>
       <c r="F50">
-        <v>1277.1490169095728</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+        <v>165.29580000000001</v>
+      </c>
+      <c r="G50">
+        <v>153.33340000000001</v>
+      </c>
+      <c r="H50">
+        <v>152.05240000000001</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="0"/>
+        <v>1031.2457999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="8">
         <v>36061</v>
       </c>
       <c r="C51">
-        <v>491.1615411462285</v>
+        <v>195.54750000000001</v>
       </c>
       <c r="D51">
-        <v>400.55005560273872</v>
+        <v>204.94220000000001</v>
       </c>
       <c r="E51">
-        <v>391.2535887914994</v>
+        <v>176.28550000000001</v>
       </c>
       <c r="F51">
-        <v>1282.9651855404666</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+        <v>163.57939999999999</v>
+      </c>
+      <c r="G51">
+        <v>151.3569</v>
+      </c>
+      <c r="H51">
+        <v>149.34110000000001</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="0"/>
+        <v>1041.0526</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="8">
         <v>36089</v>
       </c>
       <c r="C52">
-        <v>469.09005317545797</v>
+        <v>186.56540000000001</v>
       </c>
       <c r="D52">
-        <v>402.68280786464663</v>
+        <v>192.9024</v>
       </c>
       <c r="E52">
-        <v>391.92024489501409</v>
+        <v>175.27930000000001</v>
       </c>
       <c r="F52">
-        <v>1263.6931059351189</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+        <v>164.92310000000001</v>
+      </c>
+      <c r="G52">
+        <v>152.1026</v>
+      </c>
+      <c r="H52">
+        <v>150.80090000000001</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="0"/>
+        <v>1022.5736999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="8">
         <v>36137</v>
       </c>
       <c r="C53">
-        <v>396.60917033313638</v>
+        <v>141.36580000000001</v>
       </c>
       <c r="D53">
-        <v>396.43286975622379</v>
+        <v>169.87379999999999</v>
       </c>
       <c r="E53">
-        <v>384.76236745831119</v>
+        <v>169.0155</v>
       </c>
       <c r="F53">
-        <v>1177.8044075476714</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+        <v>162.38319999999999</v>
+      </c>
+      <c r="G53">
+        <v>150.40369999999999</v>
+      </c>
+      <c r="H53">
+        <v>147.5077</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="0"/>
+        <v>940.54969999999992</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="8">
         <v>36151</v>
       </c>
       <c r="C54">
-        <v>384.77426319744575</v>
+        <v>142.95650000000001</v>
       </c>
       <c r="D54">
-        <v>391.57720998790103</v>
+        <v>159.60560000000001</v>
       </c>
       <c r="E54">
-        <v>382.92182406688158</v>
+        <v>163.435</v>
       </c>
       <c r="F54">
-        <v>1159.2732972522285</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+        <v>160.05760000000001</v>
+      </c>
+      <c r="G54">
+        <v>150.29669999999999</v>
+      </c>
+      <c r="H54">
+        <v>147.5831</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="0"/>
+        <v>923.93450000000007</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="8">
         <v>36185</v>
       </c>
       <c r="C55">
-        <v>364.72820384415354</v>
+        <v>138.583</v>
       </c>
       <c r="D55">
-        <v>391.18786442284727</v>
+        <v>147.6662</v>
       </c>
       <c r="E55">
-        <v>387.6119822490125</v>
+        <v>158.17060000000001</v>
       </c>
       <c r="F55">
-        <v>1143.5280505160131</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+        <v>160.19110000000001</v>
+      </c>
+      <c r="G55">
+        <v>151.30510000000001</v>
+      </c>
+      <c r="H55">
+        <v>148.74010000000001</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>904.65610000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="8">
         <v>36216</v>
       </c>
       <c r="C56">
-        <v>335.86918506590075</v>
+        <v>118.206</v>
       </c>
       <c r="D56">
-        <v>391.62439734371014</v>
+        <v>141.27680000000001</v>
       </c>
       <c r="E56">
-        <v>390.61698924582822</v>
+        <v>154.93819999999999</v>
       </c>
       <c r="F56">
-        <v>1118.1105716554391</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+        <v>159.8244</v>
+      </c>
+      <c r="G56">
+        <v>153.24809999999999</v>
+      </c>
+      <c r="H56">
+        <v>150.5565</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="0"/>
+        <v>878.05000000000007</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="8">
         <v>36237</v>
       </c>
       <c r="C57">
-        <v>336.1342534583232</v>
+        <v>121.97969999999999</v>
       </c>
       <c r="D57">
-        <v>385.8421452623013</v>
+        <v>138.96879999999999</v>
       </c>
       <c r="E57">
-        <v>382.89598365167205</v>
+        <v>152.75280000000001</v>
       </c>
       <c r="F57">
-        <v>1104.8723823722964</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+        <v>158.208</v>
+      </c>
+      <c r="G57">
+        <v>150.06710000000001</v>
+      </c>
+      <c r="H57">
+        <v>146.8468</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="0"/>
+        <v>868.82319999999993</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>8</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="8">
         <v>36273</v>
       </c>
       <c r="C58">
-        <v>409.12454798783125</v>
+        <v>160.977</v>
       </c>
       <c r="D58">
-        <v>396.96024772696705</v>
+        <v>168.08109999999999</v>
       </c>
       <c r="E58">
-        <v>395.88494955528694</v>
+        <v>159.78659999999999</v>
       </c>
       <c r="F58">
-        <v>1201.9697452700852</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+        <v>162.2499</v>
+      </c>
+      <c r="G58">
+        <v>154.99019999999999</v>
+      </c>
+      <c r="H58">
+        <v>151.6609</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="0"/>
+        <v>957.74569999999994</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="8">
         <v>36305</v>
       </c>
       <c r="C59">
-        <v>374.72050313751788</v>
+        <v>141.0051</v>
       </c>
       <c r="D59">
-        <v>390.97815847752491</v>
+        <v>156.17939999999999</v>
       </c>
       <c r="E59">
-        <v>390.95475371698365</v>
+        <v>155.89750000000001</v>
       </c>
       <c r="F59">
-        <v>1156.6534153320265</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+        <v>159.78559999999999</v>
+      </c>
+      <c r="G59">
+        <v>152.83099999999999</v>
+      </c>
+      <c r="H59">
+        <v>150.3048</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="0"/>
+        <v>916.00340000000006</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="8">
         <v>36341</v>
       </c>
       <c r="C60">
-        <v>391.00447401320827</v>
+        <v>159.1678</v>
       </c>
       <c r="D60">
-        <v>388.74137710931223</v>
+        <v>155.01730000000001</v>
       </c>
       <c r="E60">
-        <v>391.38573617917518</v>
+        <v>154.6473</v>
       </c>
       <c r="F60">
-        <v>1171.1315873016956</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+        <v>158.58359999999999</v>
+      </c>
+      <c r="G60">
+        <v>152.32990000000001</v>
+      </c>
+      <c r="H60">
+        <v>149.41739999999999</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="0"/>
+        <v>929.16329999999994</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="8">
         <v>36369</v>
       </c>
       <c r="C61">
-        <v>404.36180310013305</v>
+        <v>169.28309999999999</v>
       </c>
       <c r="D61">
-        <v>390.34319044271399</v>
+        <v>158.22219999999999</v>
       </c>
       <c r="E61">
-        <v>394.69178186118882</v>
+        <v>154.8416</v>
       </c>
       <c r="F61">
-        <v>1189.3967754040359</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
+        <v>159.03569999999999</v>
+      </c>
+      <c r="G61">
+        <v>153.32249999999999</v>
+      </c>
+      <c r="H61">
+        <v>151.20830000000001</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="0"/>
+        <v>945.91340000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="8">
         <v>36398</v>
       </c>
       <c r="C62">
-        <v>392.89257553428678</v>
+        <v>160.84450000000001</v>
       </c>
       <c r="D62">
-        <v>387.07894840350275</v>
+        <v>155.72499999999999</v>
       </c>
       <c r="E62">
-        <v>390.68846806741357</v>
+        <v>153.7312</v>
       </c>
       <c r="F62">
-        <v>1170.6599920052031</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
+        <v>157.95519999999999</v>
+      </c>
+      <c r="G62">
+        <v>151.71549999999999</v>
+      </c>
+      <c r="H62">
+        <v>149.3511</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="0"/>
+        <v>929.32249999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="8">
         <v>36405</v>
       </c>
       <c r="C63">
-        <v>439.8928313942659</v>
+        <v>180.1009</v>
       </c>
       <c r="D63">
-        <v>392.75241918279659</v>
+        <v>176.02959999999999</v>
       </c>
       <c r="E63">
-        <v>389.99985588093284</v>
+        <v>164.66309999999999</v>
       </c>
       <c r="F63">
-        <v>1222.6451064579953</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
+        <v>159.55690000000001</v>
+      </c>
+      <c r="G63">
+        <v>152.29470000000001</v>
+      </c>
+      <c r="H63">
+        <v>148.82730000000001</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="0"/>
+        <v>981.47250000000008</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="8">
         <v>36426</v>
       </c>
       <c r="C64">
-        <v>419.16106324201138</v>
+        <v>167.8903</v>
       </c>
       <c r="D64">
-        <v>391.0585931810997</v>
+        <v>169.756</v>
       </c>
       <c r="E64">
-        <v>389.96001260483382</v>
+        <v>161.46969999999999</v>
       </c>
       <c r="F64">
-        <v>1200.1796690279448</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+        <v>159.55510000000001</v>
+      </c>
+      <c r="G64">
+        <v>151.54849999999999</v>
+      </c>
+      <c r="H64">
+        <v>149.22120000000001</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="0"/>
+        <v>959.44080000000008</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="8">
         <v>36454</v>
       </c>
       <c r="C65">
-        <v>456.62687984459154</v>
+        <v>181.10769999999999</v>
       </c>
       <c r="D65">
-        <v>402.80455674892693</v>
+        <v>186.87729999999999</v>
       </c>
       <c r="E65">
-        <v>386.6086109445331</v>
+        <v>174.14400000000001</v>
       </c>
       <c r="F65">
-        <v>1246.0400475380516</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
+        <v>164.63849999999999</v>
+      </c>
+      <c r="G65">
+        <v>152.66399999999999</v>
+      </c>
+      <c r="H65">
+        <v>148.04900000000001</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="0"/>
+        <v>1007.4805</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="8">
         <v>36482</v>
       </c>
       <c r="C66">
-        <v>492.74002557492156</v>
+        <v>197.66249999999999</v>
       </c>
       <c r="D66">
-        <v>405.37127262278409</v>
+        <v>203.1634</v>
       </c>
       <c r="E66">
-        <v>393.37017869751605</v>
+        <v>178.07419999999999</v>
       </c>
       <c r="F66">
-        <v>1291.4814768952217</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
+        <v>165.50700000000001</v>
+      </c>
+      <c r="G66">
+        <v>153.70419999999999</v>
+      </c>
+      <c r="H66">
+        <v>150.58940000000001</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="0"/>
+        <v>1048.7006999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="8">
         <v>36507</v>
       </c>
       <c r="C67">
-        <v>429.5801653125651</v>
+        <v>164.8366</v>
       </c>
       <c r="D67">
-        <v>405.17187298612572</v>
+        <v>177.05520000000001</v>
       </c>
       <c r="E67">
-        <v>393.10809122339947</v>
+        <v>172.9049</v>
       </c>
       <c r="F67">
-        <v>1227.8601295220906</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
+        <v>166.07980000000001</v>
+      </c>
+      <c r="G67">
+        <v>153.87549999999999</v>
+      </c>
+      <c r="H67">
+        <v>151.00370000000001</v>
+      </c>
+      <c r="I67">
+        <f t="shared" ref="I67:I68" si="1">SUM(C67:H67)</f>
+        <v>985.75569999999993</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="8">
         <v>36545</v>
       </c>
       <c r="C68">
-        <v>381.70792648140565</v>
+        <v>140.8501</v>
       </c>
       <c r="D68">
-        <v>397.82291436403386</v>
+        <v>159.56489999999999</v>
       </c>
       <c r="E68">
-        <v>388.26118279255968</v>
+        <v>162.96530000000001</v>
       </c>
       <c r="F68">
-        <v>1167.7920236379994</v>
+        <v>163.11609999999999</v>
+      </c>
+      <c r="G68">
+        <v>153.03460000000001</v>
+      </c>
+      <c r="H68">
+        <v>149.2936</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="1"/>
+        <v>928.82459999999992</v>
       </c>
     </row>
   </sheetData>
@@ -3000,12 +3659,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3016,7 +3675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>35307</v>
       </c>
@@ -3028,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>35344</v>
       </c>
@@ -3040,7 +3699,7 @@
         <v>18.03</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>35405</v>
       </c>
@@ -3052,7 +3711,7 @@
         <v>18.03</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>35406</v>
       </c>
@@ -3064,7 +3723,7 @@
         <v>18.03</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>35459</v>
       </c>
@@ -3076,7 +3735,7 @@
         <v>18.43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>35460</v>
       </c>
@@ -3088,7 +3747,7 @@
         <v>18.43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>35474</v>
       </c>
@@ -3100,7 +3759,7 @@
         <v>18.68</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>35834</v>
       </c>
@@ -3112,7 +3771,7 @@
         <v>19.16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>35948</v>
       </c>
@@ -3124,7 +3783,7 @@
         <v>19.16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>35968</v>
       </c>
@@ -3136,7 +3795,7 @@
         <v>19.16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>35994</v>
       </c>
@@ -3148,7 +3807,7 @@
         <v>19.16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>35996</v>
       </c>
@@ -3160,7 +3819,7 @@
         <v>23.68</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>35997</v>
       </c>
@@ -3172,7 +3831,7 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>36000</v>
       </c>
@@ -3184,7 +3843,7 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>36002</v>
       </c>
@@ -3196,7 +3855,7 @@
         <v>23.75</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>36003</v>
       </c>
@@ -3208,7 +3867,7 @@
         <v>37.76</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>36014</v>
       </c>
@@ -3220,7 +3879,7 @@
         <v>37.76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>36015</v>
       </c>
@@ -3232,7 +3891,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>36043</v>
       </c>
@@ -3244,7 +3903,7 @@
         <v>37.83</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>36050</v>
       </c>
@@ -3256,7 +3915,7 @@
         <v>37.889711133744981</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>36051</v>
       </c>
@@ -3268,7 +3927,7 @@
         <v>37.889711133744981</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>36052</v>
       </c>
@@ -3280,7 +3939,7 @@
         <v>37.889711133744981</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>36053</v>
       </c>
@@ -3292,7 +3951,7 @@
         <v>37.948488911522759</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>36056</v>
       </c>
@@ -3304,7 +3963,7 @@
         <v>38.128722244856093</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>36062</v>
       </c>
@@ -3316,7 +3975,7 @@
         <v>38.128722244856093</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>36074</v>
       </c>
@@ -3328,7 +3987,7 @@
         <v>38.228300033950802</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>36087</v>
       </c>
@@ -3340,7 +3999,7 @@
         <v>38.228300033950802</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>36088</v>
       </c>
@@ -3352,7 +4011,7 @@
         <v>38.228300033950802</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>36092</v>
       </c>
@@ -3364,7 +4023,7 @@
         <v>38.228300033950802</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>36093</v>
       </c>
@@ -3376,7 +4035,7 @@
         <v>38.228300033950802</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>36094</v>
       </c>
@@ -3388,7 +4047,7 @@
         <v>38.228300033950802</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>36096</v>
       </c>
@@ -3400,7 +4059,7 @@
         <v>38.287077811728579</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>36098</v>
       </c>
@@ -3412,7 +4071,7 @@
         <v>38.287077811728579</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>36105</v>
       </c>
@@ -3424,7 +4083,7 @@
         <v>38.287077811728579</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>36106</v>
       </c>
@@ -3436,7 +4095,7 @@
         <v>38.287077811728579</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>36107</v>
       </c>
@@ -3448,7 +4107,7 @@
         <v>38.372377811728576</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>36111</v>
       </c>
@@ -3460,7 +4119,7 @@
         <v>38.372377811728576</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>36112</v>
       </c>
@@ -3472,7 +4131,7 @@
         <v>38.372377811728576</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>36113</v>
       </c>
@@ -3484,7 +4143,7 @@
         <v>38.431155589506353</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>36116</v>
       </c>
@@ -3496,7 +4155,7 @@
         <v>42.357977834362437</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>36117</v>
       </c>
@@ -3508,7 +4167,7 @@
         <v>42.534311167695769</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>36143</v>
       </c>
@@ -3520,7 +4179,7 @@
         <v>42.534311167695769</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>36144</v>
       </c>
@@ -3532,7 +4191,7 @@
         <v>42.534311167695769</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>36149</v>
       </c>
@@ -3544,7 +4203,7 @@
         <v>42.534311167695769</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>36160</v>
       </c>
@@ -3556,7 +4215,7 @@
         <v>42.534311167695769</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>36162</v>
       </c>
@@ -3568,7 +4227,7 @@
         <v>42.534311167695769</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>36166</v>
       </c>
@@ -3580,7 +4239,7 @@
         <v>42.534311167695769</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>36168</v>
       </c>
@@ -3592,7 +4251,7 @@
         <v>42.534311167695769</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>36169</v>
       </c>
@@ -3604,7 +4263,7 @@
         <v>42.57715558950634</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>36170</v>
       </c>
@@ -3616,7 +4275,7 @@
         <v>42.694711145061895</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>36181</v>
       </c>
@@ -3628,7 +4287,7 @@
         <v>42.694711145061895</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>36183</v>
       </c>
@@ -3640,7 +4299,7 @@
         <v>42.694711145061895</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>36184</v>
       </c>
@@ -3652,7 +4311,7 @@
         <v>43.149083378601055</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>36185</v>
       </c>
@@ -3664,7 +4323,7 @@
         <v>43.149083378601055</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>36191</v>
       </c>
@@ -3676,7 +4335,7 @@
         <v>43.149083378601055</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>36192</v>
       </c>
@@ -3688,7 +4347,7 @@
         <v>43.231972267489944</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>36193</v>
       </c>
@@ -3700,7 +4359,7 @@
         <v>43.231972267489944</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>36199</v>
       </c>
@@ -3712,7 +4371,7 @@
         <v>43.231972267489944</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>36219</v>
       </c>
@@ -3724,7 +4383,7 @@
         <v>43.231972267489944</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>36220</v>
       </c>
@@ -3736,7 +4395,7 @@
         <v>43.231972267489944</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>36221</v>
       </c>
@@ -3748,7 +4407,7 @@
         <v>43.274438945473548</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>36222</v>
       </c>
@@ -3760,7 +4419,7 @@
         <v>43.274438945473548</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>36237</v>
       </c>
@@ -3772,7 +4431,7 @@
         <v>43.274438945473548</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>36238</v>
       </c>
@@ -3784,7 +4443,7 @@
         <v>43.274438945473548</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>36239</v>
       </c>
@@ -3796,7 +4455,7 @@
         <v>43.274438945473548</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>36240</v>
       </c>
@@ -3808,7 +4467,7 @@
         <v>43.274438945473548</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>36241</v>
       </c>
@@ -3820,7 +4479,7 @@
         <v>43.274438945473548</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>36242</v>
       </c>
@@ -3832,7 +4491,7 @@
         <v>43.333216723251326</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>36245</v>
       </c>
@@ -3844,7 +4503,7 @@
         <v>43.391994501029103</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>36250</v>
       </c>
@@ -3856,7 +4515,7 @@
         <v>43.391994501029103</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>36251</v>
       </c>
@@ -3868,7 +4527,7 @@
         <v>43.391994501029103</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>36252</v>
       </c>
@@ -3880,7 +4539,7 @@
         <v>43.391994501029103</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>36253</v>
       </c>
@@ -3892,7 +4551,7 @@
         <v>43.45077227880688</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>36254</v>
       </c>
@@ -3904,7 +4563,7 @@
         <v>43.45077227880688</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>36255</v>
       </c>
@@ -3916,7 +4575,7 @@
         <v>43.625261190329638</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>36293</v>
       </c>
@@ -3928,7 +4587,7 @@
         <v>43.625261190329638</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>36310</v>
       </c>
@@ -3940,7 +4599,7 @@
         <v>43.625261190329638</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>36311</v>
       </c>
@@ -3952,7 +4611,7 @@
         <v>43.625261190329638</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>36317</v>
       </c>
@@ -3964,7 +4623,7 @@
         <v>43.625261190329638</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>36318</v>
       </c>
@@ -3976,7 +4635,7 @@
         <v>43.654372301440752</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>36320</v>
       </c>
@@ -3988,7 +4647,7 @@
         <v>43.654372301440752</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>36321</v>
       </c>
@@ -4000,7 +4659,7 @@
         <v>43.701283412375034</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <v>36322</v>
       </c>
@@ -4012,7 +4671,7 @@
         <v>43.818838967930589</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
         <v>36323</v>
       </c>
@@ -4024,7 +4683,7 @@
         <v>43.877616745708366</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
         <v>36324</v>
       </c>
@@ -4036,7 +4695,7 @@
         <v>43.877616745708366</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
         <v>36325</v>
       </c>
@@ -4048,7 +4707,7 @@
         <v>43.930461190064399</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
         <v>36326</v>
       </c>
@@ -4060,7 +4719,7 @@
         <v>43.930461190064399</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="6">
         <v>36327</v>
       </c>
@@ -4072,7 +4731,7 @@
         <v>43.989238967842176</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>36341</v>
       </c>
@@ -4084,7 +4743,7 @@
         <v>43.989238967842176</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
         <v>36342</v>
       </c>
@@ -4096,7 +4755,7 @@
         <v>44.011861188649782</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>36343</v>
       </c>
@@ -4108,7 +4767,7 @@
         <v>44.070638966427559</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
         <v>36344</v>
       </c>
@@ -4120,7 +4779,7 @@
         <v>44.070638966427559</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>36412</v>
       </c>
@@ -4132,7 +4791,7 @@
         <v>44.070638966427559</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
         <v>36413</v>
       </c>
@@ -4144,7 +4803,7 @@
         <v>44.122927853901828</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
         <v>36419</v>
       </c>
@@ -4156,7 +4815,7 @@
         <v>44.122927853901828</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="6">
         <v>36420</v>
       </c>
@@ -4168,7 +4827,7 @@
         <v>44.53437229834627</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
         <v>36428</v>
       </c>
@@ -4180,7 +4839,7 @@
         <v>44.53437229834627</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
         <v>36429</v>
       </c>
@@ -4192,7 +4851,7 @@
         <v>44.69828340662815</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="6">
         <v>36435</v>
       </c>
@@ -4204,7 +4863,7 @@
         <v>44.69828340662815</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
         <v>36436</v>
       </c>
@@ -4216,7 +4875,7 @@
         <v>70.272705674118072</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>36437</v>
       </c>
@@ -4228,7 +4887,7 @@
         <v>70.384327896251875</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>36440</v>
       </c>
@@ -4240,7 +4899,7 @@
         <v>70.443105674029653</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>36441</v>
       </c>
@@ -4252,7 +4911,7 @@
         <v>70.443105674029653</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
         <v>36443</v>
       </c>
@@ -4264,7 +4923,7 @@
         <v>70.443105674029653</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>36444</v>
       </c>
@@ -4276,7 +4935,7 @@
         <v>70.507261230999831</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="6">
         <v>36447</v>
       </c>
@@ -4288,7 +4947,7 @@
         <v>70.530439007362986</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="6">
         <v>36451</v>
       </c>
@@ -4300,7 +4959,7 @@
         <v>70.530439007362986</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <v>36455</v>
       </c>
@@ -4312,7 +4971,7 @@
         <v>70.530439007362986</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="6">
         <v>36456</v>
       </c>
@@ -4324,7 +4983,7 @@
         <v>71.393572352013251</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="6">
         <v>36457</v>
       </c>
@@ -4336,7 +4995,7 @@
         <v>71.463105688175816</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
         <v>36458</v>
       </c>
@@ -4348,7 +5007,7 @@
         <v>71.58066124373137</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="6">
         <v>36459</v>
       </c>
@@ -4360,7 +5019,7 @@
         <v>71.633505688087396</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="6">
         <v>36463</v>
       </c>
@@ -4372,7 +5031,7 @@
         <v>71.633505688087396</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>36464</v>
       </c>
@@ -4384,7 +5043,7 @@
         <v>72.118194588293221</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
         <v>36465</v>
       </c>
@@ -4396,7 +5055,7 @@
         <v>72.529639032737663</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="6">
         <v>36469</v>
       </c>
@@ -4408,7 +5067,7 @@
         <v>72.635705676770456</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="6">
         <v>36470</v>
       </c>
@@ -4420,7 +5079,7 @@
         <v>82.854716765247687</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="6">
         <v>36471</v>
       </c>
@@ -4432,7 +5091,7 @@
         <v>82.913494543025465</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="6">
         <v>36472</v>
       </c>
@@ -4444,7 +5103,7 @@
         <v>82.913494543025465</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="6">
         <v>36473</v>
       </c>
@@ -4456,7 +5115,7 @@
         <v>82.913494543025465</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="6">
         <v>36479</v>
       </c>
@@ -4468,7 +5127,7 @@
         <v>82.926294554342405</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="6">
         <v>36480</v>
       </c>
@@ -4480,7 +5139,7 @@
         <v>82.985072332120183</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="6">
         <v>36485</v>
       </c>
@@ -4492,7 +5151,7 @@
         <v>82.985072332120183</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="6">
         <v>36490</v>
       </c>
@@ -4504,7 +5163,7 @@
         <v>82.985072332120183</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="6">
         <v>36498</v>
       </c>
@@ -4516,7 +5175,7 @@
         <v>82.985072332120183</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="6">
         <v>36503</v>
       </c>
@@ -4528,7 +5187,7 @@
         <v>83.129339021420719</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="6">
         <v>36504</v>
       </c>
@@ -4540,7 +5199,7 @@
         <v>83.144916796369259</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="6">
         <v>36511</v>
       </c>
@@ -4552,7 +5211,7 @@
         <v>83.144916796369259</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="6">
         <v>36517</v>
       </c>
@@ -4564,7 +5223,7 @@
         <v>83.286783508303671</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="6">
         <v>36518</v>
       </c>
@@ -4576,7 +5235,7 @@
         <v>83.353539052542288</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="6">
         <v>36519</v>
       </c>
@@ -4588,7 +5247,7 @@
         <v>83.353539052542288</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="6">
         <v>36520</v>
       </c>
@@ -4600,7 +5259,7 @@
         <v>83.382650163653395</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="6">
         <v>36521</v>
       </c>
@@ -4612,7 +5271,7 @@
         <v>83.382650163653395</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="6">
         <v>36522</v>
       </c>
@@ -4624,7 +5283,7 @@
         <v>83.638539052542285</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="6">
         <v>36523</v>
       </c>
@@ -4636,7 +5295,7 @@
         <v>83.665983496986726</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="6">
         <v>36524</v>
       </c>
@@ -4648,7 +5307,7 @@
         <v>83.665983496986726</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="6">
         <v>36528</v>
       </c>

</xml_diff>

<commit_message>
Working on perrenial crops
</commit_message>
<xml_diff>
--- a/Prototypes/Bambatsi/Observed.xlsx
+++ b/Prototypes/Bambatsi/Observed.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="39">
   <si>
     <t>B_LAI</t>
   </si>
@@ -110,7 +110,34 @@
     <t>SW100_190cm</t>
   </si>
   <si>
-    <t>SW0-190cm</t>
+    <t>Bambatsi.Root.Live.Wt</t>
+  </si>
+  <si>
+    <t>Bambatsi.Root.LengthDensity(1)</t>
+  </si>
+  <si>
+    <t>Bambatsi.Root.LengthDensity(2)</t>
+  </si>
+  <si>
+    <t>Bambatsi.Root.LengthDensity(3)</t>
+  </si>
+  <si>
+    <t>Bambatsi.Root.LengthDensity(4)</t>
+  </si>
+  <si>
+    <t>Bambatsi.Root.LengthDensity(5)</t>
+  </si>
+  <si>
+    <t>Bambatsi.Root.LengthDensity(6)</t>
+  </si>
+  <si>
+    <t>Bambatsi.Root.LengthDensity(7)</t>
+  </si>
+  <si>
+    <t>Bambatsi.Root.LengthDensity(8)</t>
+  </si>
+  <si>
+    <t>SW0_190cm</t>
   </si>
 </sst>
 </file>
@@ -558,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -575,9 +602,11 @@
     <col min="11" max="11" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="22" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -617,8 +646,35 @@
       <c r="M1" s="18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -660,7 +716,7 @@
         <v>279.125</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -702,7 +758,7 @@
         <v>464.73749928706059</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -745,7 +801,7 @@
         <v>1177.2591667905765</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -788,7 +844,7 @@
         <v>1328.827501313991</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -831,7 +887,7 @@
         <v>1328.827501313991</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -874,7 +930,7 @@
         <v>1328.827501313991</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -917,7 +973,7 @@
         <v>1465.1168150967485</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -960,7 +1016,7 @@
         <v>1642.538915422381</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1003,7 +1059,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1046,7 +1102,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1089,7 +1145,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1132,7 +1188,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1175,7 +1231,7 @@
         <v>1971.6691795607103</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1218,7 +1274,7 @@
         <v>2021.7713279289001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1261,7 +1317,7 @@
         <v>2021.7713279289001</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1304,7 +1360,7 @@
         <v>2220.7840767706889</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1347,7 +1403,7 @@
         <v>2220.7840767706889</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1390,7 +1446,7 @@
         <v>2220.7840767706889</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1433,7 +1489,7 @@
         <v>2461.4965271048768</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1476,7 +1532,7 @@
         <v>2586.6707063880876</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1519,7 +1575,7 @@
         <v>2623.7996456745291</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1562,7 +1618,7 @@
         <v>2654.7762397534466</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1605,7 +1661,7 @@
         <v>2654.7762397534466</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1648,7 +1704,7 @@
         <v>2899.8972279812174</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1691,7 +1747,7 @@
         <v>2899.8972279812174</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1710,8 +1766,26 @@
         <v>142</v>
       </c>
       <c r="M27" s="12"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>283.68413333333342</v>
+      </c>
+      <c r="O27">
+        <v>4.7491999999999993E-2</v>
+      </c>
+      <c r="P27">
+        <v>2.3890666666666664E-2</v>
+      </c>
+      <c r="Q27">
+        <v>1.8785249999999996E-2</v>
+      </c>
+      <c r="R27">
+        <v>1.31328E-2</v>
+      </c>
+      <c r="S27">
+        <v>8.7538500000000005E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1734,8 +1808,29 @@
       <c r="M28" s="13">
         <v>325.64938287832825</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>503.96834782608704</v>
+      </c>
+      <c r="O28">
+        <v>4.9755000000000001E-2</v>
+      </c>
+      <c r="P28">
+        <v>5.3909000000000006E-2</v>
+      </c>
+      <c r="Q28">
+        <v>3.6463625E-2</v>
+      </c>
+      <c r="R28">
+        <v>2.7734399999999999E-2</v>
+      </c>
+      <c r="S28">
+        <v>2.0572650000000001E-2</v>
+      </c>
+      <c r="T28">
+        <v>1.5187200000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1758,8 +1853,35 @@
       <c r="M29" s="13">
         <v>256.47388532926522</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>305.9854978723402</v>
+      </c>
+      <c r="O29">
+        <v>7.3387333333333332E-2</v>
+      </c>
+      <c r="P29">
+        <v>4.6686000000000005E-2</v>
+      </c>
+      <c r="Q29">
+        <v>1.981833333333333E-2</v>
+      </c>
+      <c r="R29">
+        <v>1.3715999999999999E-2</v>
+      </c>
+      <c r="S29">
+        <v>1.24803E-2</v>
+      </c>
+      <c r="T29">
+        <v>1.059072E-2</v>
+      </c>
+      <c r="U29">
+        <v>5.2354666666666674E-3</v>
+      </c>
+      <c r="V29">
+        <v>3.6287333333333339E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1782,8 +1904,35 @@
       <c r="M30" s="13">
         <v>1056.3668500881834</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>371.77533617021265</v>
+      </c>
+      <c r="O30">
+        <v>7.925666666666667E-2</v>
+      </c>
+      <c r="P30">
+        <v>5.5572666666666673E-2</v>
+      </c>
+      <c r="Q30">
+        <v>3.0887083333333332E-2</v>
+      </c>
+      <c r="R30">
+        <v>1.8295200000000001E-2</v>
+      </c>
+      <c r="S30">
+        <v>1.2899249999999999E-2</v>
+      </c>
+      <c r="T30">
+        <v>1.2311040000000002E-2</v>
+      </c>
+      <c r="U30">
+        <v>5.4611333333333331E-3</v>
+      </c>
+      <c r="V30">
+        <v>5.7875999999999995E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -1806,8 +1955,35 @@
       <c r="M31" s="13">
         <v>1044.5434370976257</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>380.51250000000016</v>
+      </c>
+      <c r="O31">
+        <v>7.3883333333333329E-2</v>
+      </c>
+      <c r="P31">
+        <v>5.6130666666666655E-2</v>
+      </c>
+      <c r="Q31">
+        <v>2.8631166666666666E-2</v>
+      </c>
+      <c r="R31">
+        <v>2.2852799999999996E-2</v>
+      </c>
+      <c r="S31">
+        <v>1.7287199999999999E-2</v>
+      </c>
+      <c r="T31">
+        <v>8.8927999999999993E-3</v>
+      </c>
+      <c r="U31">
+        <v>7.9208999999999998E-3</v>
+      </c>
+      <c r="V31">
+        <v>4.6851999999999996E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -1831,7 +2007,7 @@
         <v>443.97882281741386</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -1854,8 +2030,35 @@
       <c r="M33" s="13">
         <v>1010.8336461338604</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>638.59671666666668</v>
+      </c>
+      <c r="O33">
+        <v>0.113832</v>
+      </c>
+      <c r="P33">
+        <v>8.1819333333333327E-2</v>
+      </c>
+      <c r="Q33">
+        <v>5.698824999999999E-2</v>
+      </c>
+      <c r="R33">
+        <v>3.2572799999999999E-2</v>
+      </c>
+      <c r="S33">
+        <v>2.5864649999999999E-2</v>
+      </c>
+      <c r="T33">
+        <v>2.0339200000000002E-2</v>
+      </c>
+      <c r="U33">
+        <v>1.4442666666666668E-2</v>
+      </c>
+      <c r="V33">
+        <v>1.2333100000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1879,7 +2082,7 @@
         <v>1072.7916081214591</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -1899,7 +2102,7 @@
       </c>
       <c r="M35" s="15"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1922,8 +2125,29 @@
       <c r="M36" s="16">
         <v>252.21640479302832</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>496.00931111111106</v>
+      </c>
+      <c r="O36">
+        <v>5.4580666666666666E-2</v>
+      </c>
+      <c r="P36">
+        <v>4.2676666666666668E-2</v>
+      </c>
+      <c r="Q36">
+        <v>3.2552666666666667E-2</v>
+      </c>
+      <c r="R36">
+        <v>2.7712800000000003E-2</v>
+      </c>
+      <c r="S36">
+        <v>2.5600049999999999E-2</v>
+      </c>
+      <c r="T36">
+        <v>1.5321600000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -1946,8 +2170,35 @@
       <c r="M37" s="16">
         <v>114.55912803822982</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>212.56201666666669</v>
+      </c>
+      <c r="O37">
+        <v>4.3544666666666669E-2</v>
+      </c>
+      <c r="P37">
+        <v>2.2609333333333335E-2</v>
+      </c>
+      <c r="Q37">
+        <v>1.2439166666666663E-2</v>
+      </c>
+      <c r="R37">
+        <v>1.0692000000000002E-2</v>
+      </c>
+      <c r="S37">
+        <v>1.0870649999999999E-2</v>
+      </c>
+      <c r="T37">
+        <v>7.9520000000000007E-3</v>
+      </c>
+      <c r="U37">
+        <v>5.8222000000000005E-3</v>
+      </c>
+      <c r="V37">
+        <v>4.1799333333333325E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1970,8 +2221,35 @@
       <c r="M38" s="16">
         <v>489.70804761904759</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>355.83449090909096</v>
+      </c>
+      <c r="O38">
+        <v>8.0000666666666664E-2</v>
+      </c>
+      <c r="P38">
+        <v>4.1064666666666666E-2</v>
+      </c>
+      <c r="Q38">
+        <v>2.196883333333333E-2</v>
+      </c>
+      <c r="R38">
+        <v>1.5811200000000004E-2</v>
+      </c>
+      <c r="S38">
+        <v>1.1929049999999998E-2</v>
+      </c>
+      <c r="T38">
+        <v>1.27904E-2</v>
+      </c>
+      <c r="U38">
+        <v>1.181365E-2</v>
+      </c>
+      <c r="V38">
+        <v>4.823E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -1994,8 +2272,35 @@
       <c r="M39" s="16">
         <v>615.80326844810736</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>378.62602790697679</v>
+      </c>
+      <c r="O39">
+        <v>7.6693999999999998E-2</v>
+      </c>
+      <c r="P39">
+        <v>4.5838666666666666E-2</v>
+      </c>
+      <c r="Q39">
+        <v>2.3191666666666663E-2</v>
+      </c>
+      <c r="R39">
+        <v>1.6286399999999999E-2</v>
+      </c>
+      <c r="S39">
+        <v>1.844262E-2</v>
+      </c>
+      <c r="T39">
+        <v>1.365504E-2</v>
+      </c>
+      <c r="U39">
+        <v>8.9364000000000006E-3</v>
+      </c>
+      <c r="V39">
+        <v>5.7186999999999984E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -2019,7 +2324,7 @@
         <v>431.21551098074343</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -2042,8 +2347,35 @@
       <c r="M41" s="16">
         <v>952.09588616861265</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>566.45474999999999</v>
+      </c>
+      <c r="O41">
+        <v>0.10558599999999999</v>
+      </c>
+      <c r="P41">
+        <v>7.3387333333333332E-2</v>
+      </c>
+      <c r="Q41">
+        <v>4.3178666666666664E-2</v>
+      </c>
+      <c r="R41">
+        <v>2.9527199999999997E-2</v>
+      </c>
+      <c r="S41">
+        <v>2.5511850000000003E-2</v>
+      </c>
+      <c r="T41">
+        <v>1.79648E-2</v>
+      </c>
+      <c r="U41">
+        <v>1.3449733333333335E-2</v>
+      </c>
+      <c r="V41">
+        <v>1.0266099999999998E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -2079,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="M72" sqref="M72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2131,7 +2463,7 @@
         <v>28</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>